<commit_message>
New monitor for collection
</commit_message>
<xml_diff>
--- a/Postmam.xlsx
+++ b/Postmam.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="139">
   <si>
     <t>General Analysis</t>
   </si>
@@ -5771,7 +5771,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -5981,7 +5981,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -6182,7 +6182,9 @@
       <c r="F10" s="89"/>
       <c r="G10" s="89"/>
       <c r="H10" s="90"/>
-      <c r="I10" s="45"/>
+      <c r="I10" s="45" t="s">
+        <v>95</v>
+      </c>
       <c r="J10" s="37"/>
       <c r="L10" s="97" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Import a collection to a postman
</commit_message>
<xml_diff>
--- a/Postmam.xlsx
+++ b/Postmam.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="139">
   <si>
     <t>General Analysis</t>
   </si>
@@ -5771,7 +5771,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -5981,7 +5981,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -6348,7 +6348,9 @@
       <c r="F19" s="89"/>
       <c r="G19" s="89"/>
       <c r="H19" s="90"/>
-      <c r="I19" s="45"/>
+      <c r="I19" s="45" t="s">
+        <v>95</v>
+      </c>
       <c r="J19" s="37"/>
       <c r="L19" s="98" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
Add presentation questions part 1
</commit_message>
<xml_diff>
--- a/Postmam.xlsx
+++ b/Postmam.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="139">
   <si>
     <t>General Analysis</t>
   </si>
@@ -451,7 +451,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="#0.0\ &quot;h&quot;"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -610,6 +610,20 @@
       <sz val="12"/>
       <color rgb="FF666666"/>
       <name val="Inherit"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="20">
@@ -1132,7 +1146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1229,7 +1243,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1239,9 +1252,6 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1358,15 +1368,6 @@
     <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1376,18 +1377,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1411,6 +1400,28 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="19" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3890,16 +3901,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="39.950000000000003" customHeight="1">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -3919,31 +3930,31 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="47">
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="45">
         <f>E13</f>
         <v>9.1000000000000014</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="50" t="s">
+      <c r="B4" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="51">
+      <c r="D4" s="49">
         <v>43853</v>
       </c>
-      <c r="E4" s="52">
+      <c r="E4" s="50">
         <v>0.5</v>
       </c>
       <c r="F4" s="1">
@@ -3951,19 +3962,19 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="53" t="s">
+      <c r="B5" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5" s="49">
         <v>43853</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E5" s="50">
         <f>E21</f>
         <v>2</v>
       </c>
@@ -3972,36 +3983,36 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="53" t="s">
+      <c r="B6" s="47"/>
+      <c r="C6" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6" s="49">
         <v>43853</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="50">
         <f>E23</f>
         <v>3.2</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="54" t="s">
+      <c r="B7" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7" s="49">
         <v>43853</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E7" s="50">
         <v>0.5</v>
       </c>
       <c r="F7" s="1">
@@ -4009,19 +4020,19 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="55" t="s">
+      <c r="B8" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="51">
+      <c r="D8" s="49">
         <v>43853</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E8" s="50">
         <v>0.5</v>
       </c>
       <c r="F8" s="1">
@@ -4029,19 +4040,19 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="54" t="s">
+      <c r="B9" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D9" s="49">
         <v>43853</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E9" s="50">
         <v>0.2</v>
       </c>
       <c r="F9" s="1">
@@ -4049,19 +4060,19 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="54" t="s">
+      <c r="B10" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="51">
+      <c r="D10" s="49">
         <v>43853</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="50">
         <v>0.2</v>
       </c>
       <c r="F10" s="1">
@@ -4069,19 +4080,19 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="56" t="s">
+      <c r="B11" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="51">
+      <c r="D11" s="49">
         <v>43853</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="50">
         <v>1</v>
       </c>
       <c r="F11" s="1">
@@ -4089,19 +4100,19 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="55" t="s">
+      <c r="B12" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="49">
         <v>43853</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E12" s="50">
         <v>1</v>
       </c>
       <c r="F12" s="1">
@@ -4109,19 +4120,19 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1">
-      <c r="A13" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="47">
+      <c r="A13" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="45">
         <f>SUM(E4:E12)</f>
         <v>9.1000000000000014</v>
       </c>
@@ -4130,26 +4141,26 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="39.950000000000003" hidden="1" customHeight="1">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A15" s="76" t="s">
+      <c r="A15" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="47">
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="45">
         <f>E21</f>
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="44" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -4169,19 +4180,19 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="B17" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="56" t="s">
+      <c r="B17" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="51">
+      <c r="D17" s="49">
         <v>43853</v>
       </c>
-      <c r="E17" s="52">
+      <c r="E17" s="50">
         <v>0.2</v>
       </c>
       <c r="F17" s="1">
@@ -4192,19 +4203,19 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="56" t="s">
+      <c r="B18" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="51">
+      <c r="D18" s="49">
         <v>43853</v>
       </c>
-      <c r="E18" s="52">
+      <c r="E18" s="50">
         <v>0.3</v>
       </c>
       <c r="F18" s="1">
@@ -4215,19 +4226,19 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="B19" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="56" t="s">
+      <c r="B19" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="51">
+      <c r="D19" s="49">
         <v>43853</v>
       </c>
-      <c r="E19" s="52">
+      <c r="E19" s="50">
         <v>0.5</v>
       </c>
       <c r="F19" s="1">
@@ -4238,36 +4249,36 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="56" t="s">
+      <c r="B20" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="51">
+      <c r="D20" s="49">
         <v>43853</v>
       </c>
-      <c r="E20" s="52">
+      <c r="E20" s="50">
         <v>1</v>
       </c>
       <c r="F20" s="1"/>
       <c r="H20" s="31"/>
     </row>
     <row r="21" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1">
-      <c r="A21" s="57"/>
-      <c r="B21" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="47">
+      <c r="A21" s="55"/>
+      <c r="B21" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="45">
         <f>SUM(E17:E20)</f>
         <v>2</v>
       </c>
@@ -4276,26 +4287,26 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="39.950000000000003" hidden="1" customHeight="1" thickTop="1">
-      <c r="A22" s="57"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
+      <c r="A22" s="55"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
     </row>
     <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="77"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="47">
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="45">
         <f>E32</f>
         <v>3.2</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="44" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -4315,19 +4326,19 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="50" t="s">
+      <c r="B25" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="51">
+      <c r="D25" s="49">
         <v>43853</v>
       </c>
-      <c r="E25" s="52">
+      <c r="E25" s="50">
         <v>0.7</v>
       </c>
       <c r="F25" s="1">
@@ -4335,19 +4346,19 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="50" t="s">
+      <c r="B26" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="51">
+      <c r="D26" s="49">
         <v>43853</v>
       </c>
-      <c r="E26" s="52">
+      <c r="E26" s="50">
         <v>1</v>
       </c>
       <c r="F26" s="1">
@@ -4355,19 +4366,19 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="54" t="s">
+      <c r="B27" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="51">
+      <c r="D27" s="49">
         <v>43853</v>
       </c>
-      <c r="E27" s="52">
+      <c r="E27" s="50">
         <v>0.5</v>
       </c>
       <c r="F27" s="1">
@@ -4375,19 +4386,19 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="46" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="50" t="s">
+      <c r="C28" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="51">
+      <c r="D28" s="49">
         <v>43853</v>
       </c>
-      <c r="E28" s="52">
+      <c r="E28" s="50">
         <v>0.1</v>
       </c>
       <c r="F28" s="1">
@@ -4398,19 +4409,19 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="46" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="53" t="s">
+      <c r="C29" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="51">
+      <c r="D29" s="49">
         <v>43853</v>
       </c>
-      <c r="E29" s="52">
+      <c r="E29" s="50">
         <v>0.2</v>
       </c>
       <c r="F29" s="1">
@@ -4421,19 +4432,19 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="59" t="s">
+      <c r="B30" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="55" t="s">
+      <c r="C30" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="51">
+      <c r="D30" s="49">
         <v>43853</v>
       </c>
-      <c r="E30" s="52">
+      <c r="E30" s="50">
         <v>0.4</v>
       </c>
       <c r="F30" s="1">
@@ -4444,38 +4455,38 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="59" t="s">
+      <c r="B31" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="55" t="s">
+      <c r="C31" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="51">
+      <c r="D31" s="49">
         <v>43853</v>
       </c>
-      <c r="E31" s="52">
+      <c r="E31" s="50">
         <v>0.3</v>
       </c>
       <c r="F31" s="1"/>
       <c r="H31" s="32"/>
     </row>
     <row r="32" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1">
-      <c r="A32" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" s="47">
+      <c r="A32" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="45">
         <f>SUM(E25:E31)</f>
         <v>3.2</v>
       </c>
@@ -4484,26 +4495,26 @@
       </c>
     </row>
     <row r="33" spans="1:19" ht="39.950000000000003" hidden="1" customHeight="1">
-      <c r="A33" s="57"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="57"/>
+      <c r="A33" s="55"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
     </row>
     <row r="34" spans="1:19" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A34" s="79" t="s">
+      <c r="A34" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="79"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="79"/>
-      <c r="E34" s="47">
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="45">
         <f>E42</f>
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="44" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -4523,19 +4534,19 @@
       </c>
     </row>
     <row r="36" spans="1:19" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="53" t="s">
+      <c r="B36" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="51">
+      <c r="D36" s="49">
         <v>43854</v>
       </c>
-      <c r="E36" s="52">
+      <c r="E36" s="50">
         <v>1</v>
       </c>
       <c r="F36" s="1">
@@ -4543,19 +4554,19 @@
       </c>
     </row>
     <row r="37" spans="1:19" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="B37" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C37" s="53" t="s">
+      <c r="B37" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="51">
+      <c r="D37" s="49">
         <v>43854</v>
       </c>
-      <c r="E37" s="52">
+      <c r="E37" s="50">
         <v>3</v>
       </c>
       <c r="F37" s="1">
@@ -4572,19 +4583,19 @@
       </c>
     </row>
     <row r="38" spans="1:19" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="B38" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C38" s="53" t="s">
+      <c r="B38" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="51">
+      <c r="D38" s="49">
         <v>43854</v>
       </c>
-      <c r="E38" s="52">
+      <c r="E38" s="50">
         <v>2</v>
       </c>
       <c r="F38" s="1">
@@ -4595,19 +4606,19 @@
       </c>
     </row>
     <row r="39" spans="1:19" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A39" s="48" t="s">
+      <c r="A39" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="B39" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="54" t="s">
+      <c r="B39" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="51">
+      <c r="D39" s="49">
         <v>43854</v>
       </c>
-      <c r="E39" s="52">
+      <c r="E39" s="50">
         <v>1</v>
       </c>
       <c r="F39" s="1">
@@ -4618,19 +4629,19 @@
       </c>
     </row>
     <row r="40" spans="1:19" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A40" s="48" t="s">
+      <c r="A40" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="B40" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="53" t="s">
+      <c r="B40" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="51">
+      <c r="D40" s="49">
         <v>43854</v>
       </c>
-      <c r="E40" s="52" t="s">
+      <c r="E40" s="50" t="s">
         <v>76</v>
       </c>
       <c r="F40" s="1">
@@ -4641,17 +4652,17 @@
       </c>
     </row>
     <row r="41" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A41" s="48"/>
-      <c r="B41" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="50" t="s">
+      <c r="A41" s="46"/>
+      <c r="B41" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="51">
+      <c r="D41" s="49">
         <v>43847</v>
       </c>
-      <c r="E41" s="52"/>
+      <c r="E41" s="50"/>
       <c r="F41" s="1">
         <v>400503264</v>
       </c>
@@ -4669,15 +4680,15 @@
       </c>
     </row>
     <row r="42" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1">
-      <c r="A42" s="57"/>
-      <c r="B42" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="47">
+      <c r="A42" s="55"/>
+      <c r="B42" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="45">
         <f>SUM(E36:E41)</f>
         <v>7</v>
       </c>
@@ -4686,26 +4697,26 @@
       </c>
     </row>
     <row r="43" spans="1:19" ht="0.75" customHeight="1" thickTop="1">
-      <c r="A43" s="57"/>
-      <c r="B43" s="57"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
+      <c r="A43" s="55"/>
+      <c r="B43" s="55"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="55"/>
     </row>
     <row r="44" spans="1:19" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A44" s="78" t="s">
+      <c r="A44" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="78"/>
-      <c r="C44" s="78"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="47">
+      <c r="B44" s="76"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="45">
         <f>E49</f>
         <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1">
-      <c r="A45" s="46" t="s">
+      <c r="A45" s="44" t="s">
         <v>1</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -4725,19 +4736,19 @@
       </c>
     </row>
     <row r="46" spans="1:19" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A46" s="48" t="s">
+      <c r="A46" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="B46" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="54" t="s">
+      <c r="B46" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D46" s="51">
+      <c r="D46" s="49">
         <v>43854</v>
       </c>
-      <c r="E46" s="52">
+      <c r="E46" s="50">
         <v>1</v>
       </c>
       <c r="F46" s="1">
@@ -4745,19 +4756,19 @@
       </c>
     </row>
     <row r="47" spans="1:19" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A47" s="48" t="s">
+      <c r="A47" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C47" s="55" t="s">
+      <c r="B47" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D47" s="51">
+      <c r="D47" s="49">
         <v>43854</v>
       </c>
-      <c r="E47" s="52">
+      <c r="E47" s="50">
         <v>3</v>
       </c>
       <c r="F47" s="1">
@@ -4765,35 +4776,35 @@
       </c>
     </row>
     <row r="48" spans="1:19" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A48" s="48" t="s">
+      <c r="A48" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="B48" s="60"/>
-      <c r="C48" s="54" t="s">
+      <c r="B48" s="58"/>
+      <c r="C48" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="51">
+      <c r="D48" s="49">
         <v>43854</v>
       </c>
-      <c r="E48" s="52">
+      <c r="E48" s="50">
         <v>1</v>
       </c>
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1">
-      <c r="A49" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="B49" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="E49" s="47">
+      <c r="A49" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="45">
         <f>SUM(E46:E48)</f>
         <v>5</v>
       </c>
@@ -4805,10 +4816,10 @@
       <c r="A50" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="61"/>
-      <c r="C50" s="61"/>
-      <c r="D50" s="61"/>
-      <c r="E50" s="73">
+      <c r="B50" s="59"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="71">
         <f>E49+E42+E13</f>
         <v>21.1</v>
       </c>
@@ -4848,16 +4859,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="39.950000000000003" customHeight="1">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -4877,31 +4888,31 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
       <c r="E3" s="28">
         <f>E13</f>
         <v>9.1000000000000014</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="63" t="s">
+      <c r="B4" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="64">
+      <c r="D4" s="62">
         <v>43853</v>
       </c>
-      <c r="E4" s="52">
+      <c r="E4" s="50">
         <v>0.5</v>
       </c>
       <c r="F4" s="1">
@@ -4909,19 +4920,19 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="65" t="s">
+      <c r="B5" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="64">
+      <c r="D5" s="62">
         <v>43853</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E5" s="50">
         <f>E21</f>
         <v>2</v>
       </c>
@@ -4930,36 +4941,36 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="65" t="s">
+      <c r="B6" s="60"/>
+      <c r="C6" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="64">
+      <c r="D6" s="62">
         <v>43853</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="50">
         <f>E23</f>
         <v>3.2</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="66" t="s">
+      <c r="B7" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="64">
+      <c r="D7" s="62">
         <v>43853</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E7" s="50">
         <v>0.5</v>
       </c>
       <c r="F7" s="1">
@@ -4967,19 +4978,19 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="67" t="s">
+      <c r="B8" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="64">
+      <c r="D8" s="62">
         <v>43853</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E8" s="50">
         <v>0.5</v>
       </c>
       <c r="F8" s="1">
@@ -4987,19 +4998,19 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="66" t="s">
+      <c r="B9" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="62">
         <v>43853</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E9" s="50">
         <v>0.2</v>
       </c>
       <c r="F9" s="1">
@@ -5007,19 +5018,19 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="66" t="s">
+      <c r="B10" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="62">
         <v>43853</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="50">
         <v>0.2</v>
       </c>
       <c r="F10" s="1">
@@ -5027,19 +5038,19 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="68" t="s">
+      <c r="B11" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="64">
+      <c r="D11" s="62">
         <v>43853</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="50">
         <v>1</v>
       </c>
       <c r="F11" s="1">
@@ -5047,19 +5058,19 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="67" t="s">
+      <c r="B12" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="64">
+      <c r="D12" s="62">
         <v>43853</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E12" s="50">
         <v>1</v>
       </c>
       <c r="F12" s="1">
@@ -5067,19 +5078,19 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1">
-      <c r="A13" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="47">
+      <c r="A13" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="45">
         <f>SUM(E4:E12)</f>
         <v>9.1000000000000014</v>
       </c>
@@ -5088,32 +5099,32 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="39.950000000000003" hidden="1" customHeight="1">
-      <c r="A14" s="69"/>
-      <c r="B14" s="69"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="57"/>
+      <c r="A14" s="67"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="55"/>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="26"/>
-      <c r="B15" s="83" t="s">
+      <c r="B15" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
       <c r="E15" s="28">
         <f>E21</f>
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1">
-      <c r="B16" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="70" t="s">
+      <c r="B16" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="70" t="s">
+      <c r="D16" s="68" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -5124,16 +5135,16 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="68" t="s">
+      <c r="C17" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="64">
+      <c r="D17" s="62">
         <v>43853</v>
       </c>
-      <c r="E17" s="52">
+      <c r="E17" s="50">
         <v>0.2</v>
       </c>
       <c r="F17" s="1">
@@ -5144,16 +5155,16 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="68" t="s">
+      <c r="C18" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="64">
+      <c r="D18" s="62">
         <v>43853</v>
       </c>
-      <c r="E18" s="52">
+      <c r="E18" s="50">
         <v>0.3</v>
       </c>
       <c r="F18" s="1">
@@ -5164,16 +5175,16 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="C19" s="68" t="s">
+      <c r="C19" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="64">
+      <c r="D19" s="62">
         <v>43853</v>
       </c>
-      <c r="E19" s="52">
+      <c r="E19" s="50">
         <v>0.5</v>
       </c>
       <c r="F19" s="1">
@@ -5184,30 +5195,30 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="68" t="s">
+      <c r="C20" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="64">
+      <c r="D20" s="62">
         <v>43853</v>
       </c>
-      <c r="E20" s="52">
+      <c r="E20" s="50">
         <v>1</v>
       </c>
       <c r="F20" s="1"/>
       <c r="H20" s="31"/>
     </row>
     <row r="21" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1">
-      <c r="B21" s="69"/>
-      <c r="C21" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="47">
+      <c r="B21" s="67"/>
+      <c r="C21" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="45">
         <f>SUM(E17:E20)</f>
         <v>2</v>
       </c>
@@ -5216,34 +5227,34 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="39.950000000000003" hidden="1" customHeight="1" thickTop="1">
-      <c r="B22" s="69"/>
-      <c r="C22" s="69"/>
-      <c r="D22" s="69"/>
-      <c r="E22" s="57"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="55"/>
     </row>
     <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="26"/>
-      <c r="B23" s="84" t="s">
+      <c r="B23" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
+      <c r="C23" s="82"/>
+      <c r="D23" s="82"/>
       <c r="E23" s="28">
         <f>E32</f>
         <v>3.2</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1">
-      <c r="A24" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="70" t="s">
+      <c r="A24" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="70" t="s">
+      <c r="C24" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="70" t="s">
+      <c r="D24" s="68" t="s">
         <v>4</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -5254,19 +5265,19 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="63" t="s">
+      <c r="B25" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="64">
+      <c r="D25" s="62">
         <v>43853</v>
       </c>
-      <c r="E25" s="52">
+      <c r="E25" s="50">
         <v>0.7</v>
       </c>
       <c r="F25" s="1">
@@ -5274,19 +5285,19 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="63" t="s">
+      <c r="B26" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="64">
+      <c r="D26" s="62">
         <v>43853</v>
       </c>
-      <c r="E26" s="52">
+      <c r="E26" s="50">
         <v>1</v>
       </c>
       <c r="F26" s="1">
@@ -5294,19 +5305,19 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="66" t="s">
+      <c r="B27" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="64">
+      <c r="D27" s="62">
         <v>43853</v>
       </c>
-      <c r="E27" s="52">
+      <c r="E27" s="50">
         <v>0.5</v>
       </c>
       <c r="F27" s="1">
@@ -5314,19 +5325,19 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="71" t="s">
+      <c r="B28" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="63" t="s">
+      <c r="C28" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="64">
+      <c r="D28" s="62">
         <v>43853</v>
       </c>
-      <c r="E28" s="52">
+      <c r="E28" s="50">
         <v>0.1</v>
       </c>
       <c r="F28" s="1">
@@ -5337,19 +5348,19 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="71" t="s">
+      <c r="B29" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="65" t="s">
+      <c r="C29" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="64">
+      <c r="D29" s="62">
         <v>43853</v>
       </c>
-      <c r="E29" s="52">
+      <c r="E29" s="50">
         <v>0.2</v>
       </c>
       <c r="F29" s="1">
@@ -5360,19 +5371,19 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="72" t="s">
+      <c r="B30" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="67" t="s">
+      <c r="C30" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="64">
+      <c r="D30" s="62">
         <v>43853</v>
       </c>
-      <c r="E30" s="52">
+      <c r="E30" s="50">
         <v>0.4</v>
       </c>
       <c r="F30" s="1">
@@ -5383,38 +5394,38 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="72" t="s">
+      <c r="B31" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="67" t="s">
+      <c r="C31" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="64">
+      <c r="D31" s="62">
         <v>43853</v>
       </c>
-      <c r="E31" s="52">
+      <c r="E31" s="50">
         <v>0.3</v>
       </c>
       <c r="F31" s="1"/>
       <c r="H31" s="32"/>
     </row>
     <row r="32" spans="1:8" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1">
-      <c r="A32" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" s="47">
+      <c r="A32" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="45">
         <f>SUM(E25:E31)</f>
         <v>3.2</v>
       </c>
@@ -5423,35 +5434,35 @@
       </c>
     </row>
     <row r="33" spans="1:19" ht="39.950000000000003" hidden="1" customHeight="1">
-      <c r="A33" s="69"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="57"/>
+      <c r="A33" s="67"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="55"/>
     </row>
     <row r="34" spans="1:19" ht="20.100000000000001" customHeight="1">
-      <c r="A34" s="81" t="s">
+      <c r="A34" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="81"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="79"/>
       <c r="E34" s="28">
         <f>E42</f>
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1">
-      <c r="A35" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="70" t="s">
+      <c r="A35" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="70" t="s">
+      <c r="C35" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="70" t="s">
+      <c r="D35" s="68" t="s">
         <v>4</v>
       </c>
       <c r="E35" s="5" t="s">
@@ -5462,19 +5473,19 @@
       </c>
     </row>
     <row r="36" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="65" t="s">
+      <c r="B36" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="64">
+      <c r="D36" s="62">
         <v>43854</v>
       </c>
-      <c r="E36" s="52">
+      <c r="E36" s="50">
         <v>1</v>
       </c>
       <c r="F36" s="1">
@@ -5482,19 +5493,19 @@
       </c>
     </row>
     <row r="37" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="B37" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C37" s="65" t="s">
+      <c r="B37" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="64">
+      <c r="D37" s="62">
         <v>43854</v>
       </c>
-      <c r="E37" s="52">
+      <c r="E37" s="50">
         <v>3</v>
       </c>
       <c r="F37" s="1">
@@ -5511,19 +5522,19 @@
       </c>
     </row>
     <row r="38" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A38" s="69" t="s">
+      <c r="A38" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="B38" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C38" s="65" t="s">
+      <c r="B38" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="64">
+      <c r="D38" s="62">
         <v>43854</v>
       </c>
-      <c r="E38" s="52">
+      <c r="E38" s="50">
         <v>2</v>
       </c>
       <c r="F38" s="1">
@@ -5534,19 +5545,19 @@
       </c>
     </row>
     <row r="39" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A39" s="48" t="s">
+      <c r="A39" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="B39" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="66" t="s">
+      <c r="B39" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="64">
+      <c r="D39" s="62">
         <v>43854</v>
       </c>
-      <c r="E39" s="52">
+      <c r="E39" s="50">
         <v>1</v>
       </c>
       <c r="F39" s="1">
@@ -5557,19 +5568,19 @@
       </c>
     </row>
     <row r="40" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A40" s="48" t="s">
+      <c r="A40" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="B40" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="65" t="s">
+      <c r="B40" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="64">
+      <c r="D40" s="62">
         <v>43854</v>
       </c>
-      <c r="E40" s="52" t="s">
+      <c r="E40" s="50" t="s">
         <v>76</v>
       </c>
       <c r="F40" s="1">
@@ -5580,17 +5591,17 @@
       </c>
     </row>
     <row r="41" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A41" s="48"/>
-      <c r="B41" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="63" t="s">
+      <c r="A41" s="46"/>
+      <c r="B41" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="64">
+      <c r="D41" s="62">
         <v>43847</v>
       </c>
-      <c r="E41" s="52"/>
+      <c r="E41" s="50"/>
       <c r="F41" s="1">
         <v>400503264</v>
       </c>
@@ -5608,15 +5619,15 @@
       </c>
     </row>
     <row r="42" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1">
-      <c r="A42" s="69"/>
-      <c r="B42" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="69"/>
-      <c r="D42" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="47">
+      <c r="A42" s="67"/>
+      <c r="B42" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="45">
         <f>SUM(E36:E41)</f>
         <v>7</v>
       </c>
@@ -5625,26 +5636,26 @@
       </c>
     </row>
     <row r="43" spans="1:19" ht="0.75" hidden="1" customHeight="1">
-      <c r="A43" s="69"/>
-      <c r="B43" s="69"/>
-      <c r="C43" s="69"/>
-      <c r="D43" s="69"/>
-      <c r="E43" s="57"/>
+      <c r="A43" s="67"/>
+      <c r="B43" s="67"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="55"/>
     </row>
     <row r="44" spans="1:19" ht="20.100000000000001" customHeight="1">
-      <c r="A44" s="82" t="s">
+      <c r="A44" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="82"/>
-      <c r="C44" s="82"/>
-      <c r="D44" s="82"/>
+      <c r="B44" s="80"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="80"/>
       <c r="E44" s="28">
         <f>E49</f>
         <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1">
-      <c r="A45" s="46" t="s">
+      <c r="A45" s="44" t="s">
         <v>1</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -5664,19 +5675,19 @@
       </c>
     </row>
     <row r="46" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A46" s="48" t="s">
+      <c r="A46" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="B46" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="54" t="s">
+      <c r="B46" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D46" s="51">
+      <c r="D46" s="49">
         <v>43854</v>
       </c>
-      <c r="E46" s="52">
+      <c r="E46" s="50">
         <v>1</v>
       </c>
       <c r="F46" s="1">
@@ -5684,19 +5695,19 @@
       </c>
     </row>
     <row r="47" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A47" s="48" t="s">
+      <c r="A47" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C47" s="55" t="s">
+      <c r="B47" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D47" s="51">
+      <c r="D47" s="49">
         <v>43854</v>
       </c>
-      <c r="E47" s="52">
+      <c r="E47" s="50">
         <v>3</v>
       </c>
       <c r="F47" s="1">
@@ -5704,35 +5715,35 @@
       </c>
     </row>
     <row r="48" spans="1:19" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A48" s="48" t="s">
+      <c r="A48" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="B48" s="60"/>
-      <c r="C48" s="54" t="s">
+      <c r="B48" s="58"/>
+      <c r="C48" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="51">
+      <c r="D48" s="49">
         <v>43854</v>
       </c>
-      <c r="E48" s="52">
+      <c r="E48" s="50">
         <v>1</v>
       </c>
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" ht="20.100000000000001" hidden="1" customHeight="1" thickTop="1">
-      <c r="A49" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="B49" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="E49" s="47">
+      <c r="A49" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="45">
         <f>SUM(E46:E48)</f>
         <v>5</v>
       </c>
@@ -5744,10 +5755,10 @@
       <c r="A50" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="61"/>
-      <c r="C50" s="61"/>
-      <c r="D50" s="61"/>
-      <c r="E50" s="73">
+      <c r="B50" s="59"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="71">
         <f>E49+E42+E13</f>
         <v>21.1</v>
       </c>
@@ -5776,199 +5787,199 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="105"/>
-    <col min="2" max="2" width="14.625" style="100" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.75" style="100" customWidth="1"/>
-    <col min="4" max="4" width="15.125" style="100" customWidth="1"/>
-    <col min="5" max="6" width="16.375" style="100" customWidth="1"/>
-    <col min="7" max="16384" width="11" style="100"/>
+    <col min="1" max="1" width="11" style="94"/>
+    <col min="2" max="2" width="14.625" style="89" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.75" style="89" customWidth="1"/>
+    <col min="4" max="4" width="15.125" style="89" customWidth="1"/>
+    <col min="5" max="6" width="16.375" style="89" customWidth="1"/>
+    <col min="7" max="16384" width="11" style="89"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="106"/>
-      <c r="B1" s="107" t="s">
+      <c r="A1" s="95"/>
+      <c r="B1" s="96" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="107" t="s">
+      <c r="C1" s="96" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="107" t="s">
+      <c r="D1" s="96" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="107" t="s">
+      <c r="E1" s="96" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="108"/>
+      <c r="F1" s="97"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="103" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37"/>
+      <c r="C2" s="92" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="110"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="101" t="s">
+      <c r="A3" s="99"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="90" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="101" t="s">
+      <c r="D3" s="90" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="101" t="s">
+      <c r="E3" s="90" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="37"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="110"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="101" t="s">
+      <c r="A4" s="99"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="90" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="90" t="s">
         <v>136</v>
       </c>
-      <c r="E4" s="101" t="s">
+      <c r="E4" s="90" t="s">
         <v>137</v>
       </c>
-      <c r="F4" s="37"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="110"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="101" t="s">
+      <c r="A5" s="99"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="90" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="101" t="s">
+      <c r="D5" s="90" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="1:6" ht="57">
-      <c r="A6" s="110"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="104" t="s">
+      <c r="A6" s="99"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="93" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="109" t="s">
+      <c r="A7" s="98" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="90" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="101" t="s">
+      <c r="C7" s="90" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="101" t="s">
+      <c r="D7" s="90" t="s">
         <v>125</v>
       </c>
-      <c r="E7" s="101" t="s">
+      <c r="E7" s="90" t="s">
         <v>130</v>
       </c>
-      <c r="F7" s="37"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="109"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="101" t="s">
+      <c r="A8" s="98"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="111"/>
+      <c r="F8" s="100"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="110"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="101" t="s">
+      <c r="A9" s="99"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="90" t="s">
         <v>126</v>
       </c>
-      <c r="F9" s="111"/>
+      <c r="F9" s="100"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="110"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="101" t="s">
+      <c r="A10" s="99"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="90" t="s">
         <v>127</v>
       </c>
-      <c r="F10" s="111"/>
+      <c r="F10" s="100"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="110"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="101" t="s">
+      <c r="A11" s="99"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="90" t="s">
         <v>128</v>
       </c>
-      <c r="F11" s="111"/>
+      <c r="F11" s="100"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="110"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="101" t="s">
+      <c r="A12" s="99"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="90" t="s">
         <v>129</v>
       </c>
-      <c r="F12" s="111"/>
+      <c r="F12" s="100"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="109" t="s">
+      <c r="A13" s="98" t="s">
         <v>113</v>
       </c>
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="90" t="s">
         <v>105</v>
       </c>
-      <c r="C13" s="101" t="s">
+      <c r="C13" s="90" t="s">
         <v>105</v>
       </c>
-      <c r="D13" s="101" t="s">
+      <c r="D13" s="90" t="s">
         <v>132</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="109" t="s">
+      <c r="A14" s="98" t="s">
         <v>120</v>
       </c>
-      <c r="B14" s="101" t="s">
+      <c r="B14" s="90" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1">
-      <c r="A15" s="112"/>
-      <c r="B15" s="113" t="s">
+      <c r="A15" s="101"/>
+      <c r="B15" s="102" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="40"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5981,7 +5992,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection sqref="A1:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -5992,414 +6003,416 @@
     <col min="10" max="10" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1">
-      <c r="A1" s="94" t="s">
+    <row r="1" spans="1:12" ht="18.75" thickBot="1">
+      <c r="A1" s="103" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="96"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="105"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="41"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="43"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="42"/>
     </row>
     <row r="3" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A3" s="35"/>
-      <c r="B3" s="34" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="106" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="44" t="s">
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="110" t="s">
         <v>94</v>
       </c>
-      <c r="J3" s="37"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="4" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A4" s="35"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="33">
         <v>1</v>
       </c>
-      <c r="C4" s="88" t="str">
+      <c r="C4" s="83" t="str">
         <f>L4</f>
         <v>Create a clear and orderly directory structure</v>
       </c>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="45" t="s">
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="J4" s="37"/>
-      <c r="L4" s="97" t="s">
+      <c r="J4" s="36"/>
+      <c r="L4" s="86" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A5" s="35"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="33">
         <v>2</v>
       </c>
-      <c r="C5" s="88" t="str">
+      <c r="C5" s="83" t="str">
         <f t="shared" ref="C5:C11" si="0">L5</f>
         <v>Both the code and the comments must be written in English</v>
       </c>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="45" t="s">
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="J5" s="37"/>
-      <c r="L5" s="97" t="s">
+      <c r="J5" s="36"/>
+      <c r="L5" s="86" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A6" s="35"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="33">
         <v>3</v>
       </c>
-      <c r="C6" s="88" t="str">
+      <c r="C6" s="83" t="str">
         <f t="shared" si="0"/>
         <v>Use the camelCase code style to define variables and functions</v>
       </c>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="89"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="45" t="s">
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="J6" s="37"/>
-      <c r="L6" s="97" t="s">
+      <c r="J6" s="36"/>
+      <c r="L6" s="86" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="18" customHeight="1">
-      <c r="A7" s="35"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="33">
         <v>4</v>
       </c>
-      <c r="C7" s="88" t="str">
+      <c r="C7" s="83" t="str">
         <f t="shared" si="0"/>
         <v>In the case of using HTML, never use online styles</v>
       </c>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="89"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="45" t="s">
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="J7" s="37"/>
-      <c r="L7" s="97" t="s">
+      <c r="J7" s="36"/>
+      <c r="L7" s="86" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A8" s="35"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="33">
         <v>5</v>
       </c>
-      <c r="C8" s="88" t="str">
+      <c r="C8" s="83" t="str">
         <f t="shared" si="0"/>
         <v>In the case of using different programming languages ​​always define the implementation in separate terms</v>
       </c>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="45" t="s">
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="J8" s="37"/>
-      <c r="L8" s="97" t="s">
+      <c r="J8" s="36"/>
+      <c r="L8" s="86" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="32.25" customHeight="1">
-      <c r="A9" s="35"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="33">
         <v>6</v>
       </c>
-      <c r="C9" s="88" t="str">
+      <c r="C9" s="83" t="str">
         <f t="shared" si="0"/>
         <v>Remember that it is important to divide the tasks into several sub-tasks so that in this way you can associate each particular step of the construction with a specific commit</v>
       </c>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="45" t="s">
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="J9" s="37"/>
-      <c r="L9" s="97" t="s">
+      <c r="J9" s="36"/>
+      <c r="L9" s="86" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="31.5" customHeight="1">
-      <c r="A10" s="35"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="33">
         <v>7</v>
       </c>
-      <c r="C10" s="88" t="str">
+      <c r="C10" s="83" t="str">
         <f t="shared" si="0"/>
         <v>You should try as much as possible that the commits and the planned tasks are the same</v>
       </c>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="45" t="s">
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="J10" s="37"/>
-      <c r="L10" s="97" t="s">
+      <c r="J10" s="36"/>
+      <c r="L10" s="86" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="45.75" customHeight="1">
-      <c r="A11" s="35"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="33">
         <v>8</v>
       </c>
-      <c r="C11" s="88" t="str">
+      <c r="C11" s="83" t="str">
         <f t="shared" si="0"/>
         <v>Delete files that are not used or are not necessary to evaluate the project</v>
       </c>
-      <c r="D11" s="89"/>
-      <c r="E11" s="89"/>
-      <c r="F11" s="89"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="45" t="s">
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="84"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="J11" s="37"/>
-      <c r="L11" s="97" t="s">
+      <c r="J11" s="36"/>
+      <c r="L11" s="86" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A12" s="38"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="40"/>
-    </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1">
-      <c r="A13" s="85" t="s">
+      <c r="A12" s="37"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="39"/>
+    </row>
+    <row r="13" spans="1:12" ht="18.75" thickBot="1">
+      <c r="A13" s="103" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="87"/>
+      <c r="B13" s="104"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="104"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="104"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="105"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="35"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="37"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="36"/>
     </row>
     <row r="15" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A15" s="35"/>
-      <c r="B15" s="34" t="s">
+      <c r="A15" s="34"/>
+      <c r="B15" s="106" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="91" t="s">
+      <c r="C15" s="107" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="92"/>
-      <c r="E15" s="92"/>
-      <c r="F15" s="92"/>
-      <c r="G15" s="92"/>
-      <c r="H15" s="93"/>
-      <c r="I15" s="44" t="s">
+      <c r="D15" s="108"/>
+      <c r="E15" s="108"/>
+      <c r="F15" s="108"/>
+      <c r="G15" s="108"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="110" t="s">
         <v>94</v>
       </c>
-      <c r="J15" s="37"/>
+      <c r="J15" s="36"/>
     </row>
     <row r="16" spans="1:12" ht="15">
-      <c r="A16" s="35"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="33">
         <v>1</v>
       </c>
-      <c r="C16" s="88" t="str">
+      <c r="C16" s="83" t="str">
         <f>L16</f>
         <v>Repository with all project files</v>
       </c>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="89"/>
-      <c r="H16" s="90"/>
-      <c r="I16" s="45" t="s">
+      <c r="D16" s="84"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="J16" s="37"/>
-      <c r="L16" s="98" t="s">
+      <c r="J16" s="36"/>
+      <c r="L16" s="87" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A17" s="35"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="33">
         <v>2</v>
       </c>
-      <c r="C17" s="88" t="str">
+      <c r="C17" s="83" t="str">
         <f>L17</f>
         <v>You must create a correctly documented README file in the root directory of the project (see guidelines in Resources)</v>
       </c>
-      <c r="D17" s="89"/>
-      <c r="E17" s="89"/>
-      <c r="F17" s="89"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="90"/>
-      <c r="I17" s="45" t="s">
+      <c r="D17" s="84"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="85"/>
+      <c r="I17" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="J17" s="37"/>
-      <c r="L17" s="98" t="s">
+      <c r="J17" s="36"/>
+      <c r="L17" s="87" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15">
-      <c r="A18" s="35"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="33">
         <v>3</v>
       </c>
-      <c r="C18" s="88" t="str">
+      <c r="C18" s="83" t="str">
         <f>L18</f>
         <v>Documentation of the pill in PDF format</v>
       </c>
-      <c r="D18" s="89"/>
-      <c r="E18" s="89"/>
-      <c r="F18" s="89"/>
-      <c r="G18" s="89"/>
-      <c r="H18" s="90"/>
-      <c r="I18" s="45" t="s">
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="84"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="J18" s="37"/>
-      <c r="L18" s="98" t="s">
+      <c r="J18" s="36"/>
+      <c r="L18" s="87" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15">
-      <c r="A19" s="35"/>
+      <c r="A19" s="34"/>
       <c r="B19" s="33">
         <v>4</v>
       </c>
-      <c r="C19" s="88" t="str">
+      <c r="C19" s="83" t="str">
         <f>L19</f>
         <v>Presentation of the pill in PDF format</v>
       </c>
-      <c r="D19" s="89"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="90"/>
-      <c r="I19" s="45" t="s">
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="85"/>
+      <c r="I19" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="J19" s="37"/>
-      <c r="L19" s="98" t="s">
+      <c r="J19" s="36"/>
+      <c r="L19" s="87" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15">
-      <c r="A20" s="35"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="33">
         <v>5</v>
       </c>
-      <c r="C20" s="88" t="str">
+      <c r="C20" s="83" t="str">
         <f>L20</f>
         <v>POSTMAN collection into the project repository</v>
       </c>
-      <c r="D20" s="89"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="90"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="37"/>
-      <c r="L20" s="98" t="s">
+      <c r="D20" s="84"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="84"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="J20" s="36"/>
+      <c r="L20" s="87" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A21" s="38"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="40"/>
-      <c r="L21" s="98"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="39"/>
+      <c r="L21" s="87"/>
     </row>
     <row r="22" spans="1:12" ht="15">
-      <c r="L22" s="98"/>
+      <c r="L22" s="87"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="L23" s="99"/>
+      <c r="L23" s="88"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="L24" s="99"/>
+      <c r="L24" s="88"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="L25" s="99"/>
+      <c r="L25" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="17">

</xml_diff>